<commit_message>
Final Code chnage of Bundle testcase using Excel
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/AddProductData.xlsx
+++ b/data/BigCommerceData/AddProductData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Big C automation\FinReconProj\data\BigCommerceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69391130-72EE-467F-BDBD-19AD5770C3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811F4B50-3817-4ADC-91E7-5560DC9DDAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C83B9D-FCEB-4855-8FAE-05F93CD7020C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>productName</t>
   </si>
@@ -198,10 +198,34 @@
     <t>comptia-itf-logo.png</t>
   </si>
   <si>
-    <t>Comptia Product 8 Voucher</t>
-  </si>
-  <si>
-    <t>CP-1008</t>
+    <t>Modifier name</t>
+  </si>
+  <si>
+    <t>Test001, Test002</t>
+  </si>
+  <si>
+    <t>Modifier Type</t>
+  </si>
+  <si>
+    <t>Modifier Value</t>
+  </si>
+  <si>
+    <t>Test prodouct client voucher, Test product key - fulfilled ebook - component</t>
+  </si>
+  <si>
+    <t>Dropdown, Dropdown</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Yes, No</t>
+  </si>
+  <si>
+    <t>Comptia Product 54 Voucher</t>
+  </si>
+  <si>
+    <t>CP-1054</t>
   </si>
 </sst>
 </file>
@@ -254,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -264,6 +288,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -580,15 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5408E5AC-DCB9-483F-BE95-32B1B2129EFD}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,13 +727,25 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2">
         <v>49.99</v>
@@ -812,6 +851,18 @@
       </c>
       <c r="AK2" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>